<commit_message>
se reemplazo la ventana emergente con una ventana bloqueante info_procesos
</commit_message>
<xml_diff>
--- a/Otros/Gantt-G1.xlsx
+++ b/Otros/Gantt-G1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A632470-98BE-4C14-BEA1-2CC93299FDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AB4259-5BDC-44EF-9242-F32B9F788162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="-120" windowWidth="19410" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="-120" windowWidth="19545" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -2358,7 +2358,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
+      <selection pane="bottomLeft" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2423,8 +2423,8 @@
       </c>
       <c r="F3" s="82"/>
       <c r="G3" s="83">
-        <f ca="1">TODAY()</f>
-        <v>44740</v>
+        <f>DATEVALUE("1/07/2022")</f>
+        <v>44743</v>
       </c>
       <c r="H3" s="84"/>
     </row>
@@ -2440,7 +2440,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="78">
-        <f ca="1">K5</f>
+        <f>K5</f>
         <v>44739</v>
       </c>
       <c r="L4" s="79"/>
@@ -2450,7 +2450,7 @@
       <c r="P4" s="79"/>
       <c r="Q4" s="80"/>
       <c r="R4" s="78">
-        <f ca="1">R5</f>
+        <f>R5</f>
         <v>44746</v>
       </c>
       <c r="S4" s="79"/>
@@ -2460,7 +2460,7 @@
       <c r="W4" s="79"/>
       <c r="X4" s="80"/>
       <c r="Y4" s="78">
-        <f ca="1">Y5</f>
+        <f>Y5</f>
         <v>44753</v>
       </c>
       <c r="Z4" s="79"/>
@@ -2470,7 +2470,7 @@
       <c r="AD4" s="79"/>
       <c r="AE4" s="80"/>
       <c r="AF4" s="78">
-        <f ca="1">AF5</f>
+        <f>AF5</f>
         <v>44760</v>
       </c>
       <c r="AG4" s="79"/>
@@ -2480,7 +2480,7 @@
       <c r="AK4" s="79"/>
       <c r="AL4" s="80"/>
       <c r="AM4" s="78">
-        <f ca="1">AM5</f>
+        <f>AM5</f>
         <v>44767</v>
       </c>
       <c r="AN4" s="79"/>
@@ -2490,7 +2490,7 @@
       <c r="AR4" s="79"/>
       <c r="AS4" s="80"/>
       <c r="AT4" s="78">
-        <f ca="1">AT5</f>
+        <f>AT5</f>
         <v>44774</v>
       </c>
       <c r="AU4" s="79"/>
@@ -2500,7 +2500,7 @@
       <c r="AY4" s="79"/>
       <c r="AZ4" s="80"/>
       <c r="BA4" s="78">
-        <f ca="1">BA5</f>
+        <f>BA5</f>
         <v>44781</v>
       </c>
       <c r="BB4" s="79"/>
@@ -2510,7 +2510,7 @@
       <c r="BF4" s="79"/>
       <c r="BG4" s="80"/>
       <c r="BH4" s="78">
-        <f ca="1">BH5</f>
+        <f>BH5</f>
         <v>44788</v>
       </c>
       <c r="BI4" s="79"/>
@@ -2520,7 +2520,7 @@
       <c r="BM4" s="79"/>
       <c r="BN4" s="80"/>
       <c r="BO4" s="78">
-        <f ca="1">BO5</f>
+        <f>BO5</f>
         <v>44795</v>
       </c>
       <c r="BP4" s="79"/>
@@ -2530,7 +2530,7 @@
       <c r="BT4" s="79"/>
       <c r="BU4" s="80"/>
       <c r="BV4" s="78">
-        <f ca="1">BV5</f>
+        <f>BV5</f>
         <v>44802</v>
       </c>
       <c r="BW4" s="79"/>
@@ -2540,7 +2540,7 @@
       <c r="CA4" s="79"/>
       <c r="CB4" s="80"/>
       <c r="CC4" s="78">
-        <f ca="1">CC5</f>
+        <f>CC5</f>
         <v>44809</v>
       </c>
       <c r="CD4" s="79"/>
@@ -2550,7 +2550,7 @@
       <c r="CH4" s="79"/>
       <c r="CI4" s="80"/>
       <c r="CJ4" s="78">
-        <f ca="1">CJ5</f>
+        <f>CJ5</f>
         <v>44816</v>
       </c>
       <c r="CK4" s="79"/>
@@ -2560,7 +2560,7 @@
       <c r="CO4" s="79"/>
       <c r="CP4" s="80"/>
       <c r="CQ4" s="78">
-        <f ca="1">CQ5</f>
+        <f>CQ5</f>
         <v>44823</v>
       </c>
       <c r="CR4" s="79"/>
@@ -2570,7 +2570,7 @@
       <c r="CV4" s="79"/>
       <c r="CW4" s="80"/>
       <c r="CX4" s="78">
-        <f ca="1">CX5</f>
+        <f>CX5</f>
         <v>44830</v>
       </c>
       <c r="CY4" s="79"/>
@@ -2580,7 +2580,7 @@
       <c r="DC4" s="79"/>
       <c r="DD4" s="80"/>
       <c r="DE4" s="78">
-        <f ca="1">DE5</f>
+        <f>DE5</f>
         <v>44837</v>
       </c>
       <c r="DF4" s="79"/>
@@ -2590,7 +2590,7 @@
       <c r="DJ4" s="79"/>
       <c r="DK4" s="80"/>
       <c r="DL4" s="78">
-        <f ca="1">DL5</f>
+        <f>DL5</f>
         <v>44844</v>
       </c>
       <c r="DM4" s="79"/>
@@ -2600,7 +2600,7 @@
       <c r="DQ4" s="79"/>
       <c r="DR4" s="80"/>
       <c r="DS4" s="78">
-        <f ca="1">DS5</f>
+        <f>DS5</f>
         <v>44851</v>
       </c>
       <c r="DT4" s="79"/>
@@ -2610,7 +2610,7 @@
       <c r="DX4" s="79"/>
       <c r="DY4" s="80"/>
       <c r="DZ4" s="78">
-        <f ca="1">DZ5</f>
+        <f>DZ5</f>
         <v>44858</v>
       </c>
       <c r="EA4" s="79"/>
@@ -2620,7 +2620,7 @@
       <c r="EE4" s="79"/>
       <c r="EF4" s="80"/>
       <c r="EG4" s="78">
-        <f ca="1">EG5</f>
+        <f>EG5</f>
         <v>44865</v>
       </c>
       <c r="EH4" s="79"/>
@@ -2630,7 +2630,7 @@
       <c r="EL4" s="79"/>
       <c r="EM4" s="80"/>
       <c r="EN4" s="78">
-        <f ca="1">EN5</f>
+        <f>EN5</f>
         <v>44872</v>
       </c>
       <c r="EO4" s="79"/>
@@ -2640,7 +2640,7 @@
       <c r="ES4" s="79"/>
       <c r="ET4" s="80"/>
       <c r="EU4" s="78">
-        <f ca="1">EU5</f>
+        <f>EU5</f>
         <v>44879</v>
       </c>
       <c r="EV4" s="79"/>
@@ -2663,591 +2663,591 @@
       <c r="H5" s="53"/>
       <c r="I5" s="53"/>
       <c r="K5" s="68">
-        <f ca="1">Inicio_del_proyecto-WEEKDAY(Inicio_del_proyecto,1)+2+7*(Semana_para_mostrar-1)</f>
+        <f>Inicio_del_proyecto-WEEKDAY(Inicio_del_proyecto,1)+2+7*(Semana_para_mostrar-1)</f>
         <v>44739</v>
       </c>
       <c r="L5" s="69">
-        <f ca="1">K5+1</f>
+        <f>K5+1</f>
         <v>44740</v>
       </c>
       <c r="M5" s="69">
-        <f t="shared" ref="M5:AZ5" ca="1" si="0">L5+1</f>
+        <f t="shared" ref="M5:AZ5" si="0">L5+1</f>
         <v>44741</v>
       </c>
       <c r="N5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44742</v>
       </c>
       <c r="O5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44743</v>
       </c>
       <c r="P5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44744</v>
       </c>
       <c r="Q5" s="70">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44745</v>
       </c>
       <c r="R5" s="68">
-        <f ca="1">Q5+1</f>
+        <f>Q5+1</f>
         <v>44746</v>
       </c>
       <c r="S5" s="69">
-        <f ca="1">R5+1</f>
+        <f>R5+1</f>
         <v>44747</v>
       </c>
       <c r="T5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44748</v>
       </c>
       <c r="U5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44749</v>
       </c>
       <c r="V5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44750</v>
       </c>
       <c r="W5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44751</v>
       </c>
       <c r="X5" s="70">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44752</v>
       </c>
       <c r="Y5" s="68">
-        <f ca="1">X5+1</f>
+        <f>X5+1</f>
         <v>44753</v>
       </c>
       <c r="Z5" s="69">
-        <f ca="1">Y5+1</f>
+        <f>Y5+1</f>
         <v>44754</v>
       </c>
       <c r="AA5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44755</v>
       </c>
       <c r="AB5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44756</v>
       </c>
       <c r="AC5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44757</v>
       </c>
       <c r="AD5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44758</v>
       </c>
       <c r="AE5" s="70">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44759</v>
       </c>
       <c r="AF5" s="68">
-        <f ca="1">AE5+1</f>
+        <f>AE5+1</f>
         <v>44760</v>
       </c>
       <c r="AG5" s="69">
-        <f ca="1">AF5+1</f>
+        <f>AF5+1</f>
         <v>44761</v>
       </c>
       <c r="AH5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44762</v>
       </c>
       <c r="AI5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44763</v>
       </c>
       <c r="AJ5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44764</v>
       </c>
       <c r="AK5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44765</v>
       </c>
       <c r="AL5" s="70">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44766</v>
       </c>
       <c r="AM5" s="68">
-        <f ca="1">AL5+1</f>
+        <f>AL5+1</f>
         <v>44767</v>
       </c>
       <c r="AN5" s="69">
-        <f ca="1">AM5+1</f>
+        <f>AM5+1</f>
         <v>44768</v>
       </c>
       <c r="AO5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44769</v>
       </c>
       <c r="AP5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44770</v>
       </c>
       <c r="AQ5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44771</v>
       </c>
       <c r="AR5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44772</v>
       </c>
       <c r="AS5" s="70">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44773</v>
       </c>
       <c r="AT5" s="68">
-        <f ca="1">AS5+1</f>
+        <f>AS5+1</f>
         <v>44774</v>
       </c>
       <c r="AU5" s="69">
-        <f ca="1">AT5+1</f>
+        <f>AT5+1</f>
         <v>44775</v>
       </c>
       <c r="AV5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44776</v>
       </c>
       <c r="AW5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44777</v>
       </c>
       <c r="AX5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44778</v>
       </c>
       <c r="AY5" s="69">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44779</v>
       </c>
       <c r="AZ5" s="70">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" si="0"/>
         <v>44780</v>
       </c>
       <c r="BA5" s="68">
-        <f ca="1">AZ5+1</f>
+        <f>AZ5+1</f>
         <v>44781</v>
       </c>
       <c r="BB5" s="69">
-        <f ca="1">BA5+1</f>
+        <f>BA5+1</f>
         <v>44782</v>
       </c>
       <c r="BC5" s="69">
-        <f t="shared" ref="BC5:BG5" ca="1" si="1">BB5+1</f>
+        <f t="shared" ref="BC5:BG5" si="1">BB5+1</f>
         <v>44783</v>
       </c>
       <c r="BD5" s="69">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>44784</v>
       </c>
       <c r="BE5" s="69">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>44785</v>
       </c>
       <c r="BF5" s="69">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>44786</v>
       </c>
       <c r="BG5" s="70">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>44787</v>
       </c>
       <c r="BH5" s="68">
-        <f ca="1">BG5+1</f>
+        <f>BG5+1</f>
         <v>44788</v>
       </c>
       <c r="BI5" s="69">
-        <f ca="1">BH5+1</f>
+        <f>BH5+1</f>
         <v>44789</v>
       </c>
       <c r="BJ5" s="69">
-        <f t="shared" ref="BJ5:BN5" ca="1" si="2">BI5+1</f>
+        <f t="shared" ref="BJ5:BN5" si="2">BI5+1</f>
         <v>44790</v>
       </c>
       <c r="BK5" s="69">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>44791</v>
       </c>
       <c r="BL5" s="69">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>44792</v>
       </c>
       <c r="BM5" s="69">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>44793</v>
       </c>
       <c r="BN5" s="70">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" si="2"/>
         <v>44794</v>
       </c>
       <c r="BO5" s="68">
-        <f ca="1">BN5+1</f>
+        <f>BN5+1</f>
         <v>44795</v>
       </c>
       <c r="BP5" s="69">
-        <f ca="1">BO5+1</f>
+        <f>BO5+1</f>
         <v>44796</v>
       </c>
       <c r="BQ5" s="69">
-        <f t="shared" ref="BQ5" ca="1" si="3">BP5+1</f>
+        <f t="shared" ref="BQ5" si="3">BP5+1</f>
         <v>44797</v>
       </c>
       <c r="BR5" s="69">
-        <f t="shared" ref="BR5" ca="1" si="4">BQ5+1</f>
+        <f t="shared" ref="BR5" si="4">BQ5+1</f>
         <v>44798</v>
       </c>
       <c r="BS5" s="69">
-        <f t="shared" ref="BS5" ca="1" si="5">BR5+1</f>
+        <f t="shared" ref="BS5" si="5">BR5+1</f>
         <v>44799</v>
       </c>
       <c r="BT5" s="69">
-        <f t="shared" ref="BT5" ca="1" si="6">BS5+1</f>
+        <f t="shared" ref="BT5" si="6">BS5+1</f>
         <v>44800</v>
       </c>
       <c r="BU5" s="70">
-        <f t="shared" ref="BU5" ca="1" si="7">BT5+1</f>
+        <f t="shared" ref="BU5" si="7">BT5+1</f>
         <v>44801</v>
       </c>
       <c r="BV5" s="68">
-        <f ca="1">BU5+1</f>
+        <f>BU5+1</f>
         <v>44802</v>
       </c>
       <c r="BW5" s="69">
-        <f ca="1">BV5+1</f>
+        <f>BV5+1</f>
         <v>44803</v>
       </c>
       <c r="BX5" s="69">
-        <f t="shared" ref="BX5" ca="1" si="8">BW5+1</f>
+        <f t="shared" ref="BX5" si="8">BW5+1</f>
         <v>44804</v>
       </c>
       <c r="BY5" s="69">
-        <f t="shared" ref="BY5" ca="1" si="9">BX5+1</f>
+        <f t="shared" ref="BY5" si="9">BX5+1</f>
         <v>44805</v>
       </c>
       <c r="BZ5" s="69">
-        <f t="shared" ref="BZ5" ca="1" si="10">BY5+1</f>
+        <f t="shared" ref="BZ5" si="10">BY5+1</f>
         <v>44806</v>
       </c>
       <c r="CA5" s="69">
-        <f t="shared" ref="CA5" ca="1" si="11">BZ5+1</f>
+        <f t="shared" ref="CA5" si="11">BZ5+1</f>
         <v>44807</v>
       </c>
       <c r="CB5" s="70">
-        <f t="shared" ref="CB5" ca="1" si="12">CA5+1</f>
+        <f t="shared" ref="CB5" si="12">CA5+1</f>
         <v>44808</v>
       </c>
       <c r="CC5" s="68">
-        <f ca="1">CB5+1</f>
+        <f>CB5+1</f>
         <v>44809</v>
       </c>
       <c r="CD5" s="69">
-        <f ca="1">CC5+1</f>
+        <f>CC5+1</f>
         <v>44810</v>
       </c>
       <c r="CE5" s="69">
-        <f t="shared" ref="CE5" ca="1" si="13">CD5+1</f>
+        <f t="shared" ref="CE5" si="13">CD5+1</f>
         <v>44811</v>
       </c>
       <c r="CF5" s="69">
-        <f t="shared" ref="CF5" ca="1" si="14">CE5+1</f>
+        <f t="shared" ref="CF5" si="14">CE5+1</f>
         <v>44812</v>
       </c>
       <c r="CG5" s="69">
-        <f t="shared" ref="CG5" ca="1" si="15">CF5+1</f>
+        <f t="shared" ref="CG5" si="15">CF5+1</f>
         <v>44813</v>
       </c>
       <c r="CH5" s="69">
-        <f t="shared" ref="CH5" ca="1" si="16">CG5+1</f>
+        <f t="shared" ref="CH5" si="16">CG5+1</f>
         <v>44814</v>
       </c>
       <c r="CI5" s="70">
-        <f t="shared" ref="CI5" ca="1" si="17">CH5+1</f>
+        <f t="shared" ref="CI5" si="17">CH5+1</f>
         <v>44815</v>
       </c>
       <c r="CJ5" s="68">
-        <f ca="1">CI5+1</f>
+        <f>CI5+1</f>
         <v>44816</v>
       </c>
       <c r="CK5" s="69">
-        <f ca="1">CJ5+1</f>
+        <f>CJ5+1</f>
         <v>44817</v>
       </c>
       <c r="CL5" s="69">
-        <f t="shared" ref="CL5" ca="1" si="18">CK5+1</f>
+        <f t="shared" ref="CL5" si="18">CK5+1</f>
         <v>44818</v>
       </c>
       <c r="CM5" s="69">
-        <f t="shared" ref="CM5" ca="1" si="19">CL5+1</f>
+        <f t="shared" ref="CM5" si="19">CL5+1</f>
         <v>44819</v>
       </c>
       <c r="CN5" s="69">
-        <f t="shared" ref="CN5" ca="1" si="20">CM5+1</f>
+        <f t="shared" ref="CN5" si="20">CM5+1</f>
         <v>44820</v>
       </c>
       <c r="CO5" s="69">
-        <f t="shared" ref="CO5" ca="1" si="21">CN5+1</f>
+        <f t="shared" ref="CO5" si="21">CN5+1</f>
         <v>44821</v>
       </c>
       <c r="CP5" s="70">
-        <f t="shared" ref="CP5" ca="1" si="22">CO5+1</f>
+        <f t="shared" ref="CP5" si="22">CO5+1</f>
         <v>44822</v>
       </c>
       <c r="CQ5" s="68">
-        <f ca="1">CP5+1</f>
+        <f>CP5+1</f>
         <v>44823</v>
       </c>
       <c r="CR5" s="69">
-        <f ca="1">CQ5+1</f>
+        <f>CQ5+1</f>
         <v>44824</v>
       </c>
       <c r="CS5" s="69">
-        <f t="shared" ref="CS5" ca="1" si="23">CR5+1</f>
+        <f t="shared" ref="CS5" si="23">CR5+1</f>
         <v>44825</v>
       </c>
       <c r="CT5" s="69">
-        <f t="shared" ref="CT5" ca="1" si="24">CS5+1</f>
+        <f t="shared" ref="CT5" si="24">CS5+1</f>
         <v>44826</v>
       </c>
       <c r="CU5" s="69">
-        <f t="shared" ref="CU5" ca="1" si="25">CT5+1</f>
+        <f t="shared" ref="CU5" si="25">CT5+1</f>
         <v>44827</v>
       </c>
       <c r="CV5" s="69">
-        <f t="shared" ref="CV5" ca="1" si="26">CU5+1</f>
+        <f t="shared" ref="CV5" si="26">CU5+1</f>
         <v>44828</v>
       </c>
       <c r="CW5" s="70">
-        <f t="shared" ref="CW5" ca="1" si="27">CV5+1</f>
+        <f t="shared" ref="CW5" si="27">CV5+1</f>
         <v>44829</v>
       </c>
       <c r="CX5" s="68">
-        <f ca="1">CW5+1</f>
+        <f>CW5+1</f>
         <v>44830</v>
       </c>
       <c r="CY5" s="69">
-        <f ca="1">CX5+1</f>
+        <f>CX5+1</f>
         <v>44831</v>
       </c>
       <c r="CZ5" s="69">
-        <f t="shared" ref="CZ5" ca="1" si="28">CY5+1</f>
+        <f t="shared" ref="CZ5" si="28">CY5+1</f>
         <v>44832</v>
       </c>
       <c r="DA5" s="69">
-        <f t="shared" ref="DA5" ca="1" si="29">CZ5+1</f>
+        <f t="shared" ref="DA5" si="29">CZ5+1</f>
         <v>44833</v>
       </c>
       <c r="DB5" s="69">
-        <f t="shared" ref="DB5" ca="1" si="30">DA5+1</f>
+        <f t="shared" ref="DB5" si="30">DA5+1</f>
         <v>44834</v>
       </c>
       <c r="DC5" s="69">
-        <f t="shared" ref="DC5" ca="1" si="31">DB5+1</f>
+        <f t="shared" ref="DC5" si="31">DB5+1</f>
         <v>44835</v>
       </c>
       <c r="DD5" s="70">
-        <f t="shared" ref="DD5" ca="1" si="32">DC5+1</f>
+        <f t="shared" ref="DD5" si="32">DC5+1</f>
         <v>44836</v>
       </c>
       <c r="DE5" s="68">
-        <f ca="1">DD5+1</f>
+        <f>DD5+1</f>
         <v>44837</v>
       </c>
       <c r="DF5" s="69">
-        <f ca="1">DE5+1</f>
+        <f>DE5+1</f>
         <v>44838</v>
       </c>
       <c r="DG5" s="69">
-        <f t="shared" ref="DG5" ca="1" si="33">DF5+1</f>
+        <f t="shared" ref="DG5" si="33">DF5+1</f>
         <v>44839</v>
       </c>
       <c r="DH5" s="69">
-        <f t="shared" ref="DH5" ca="1" si="34">DG5+1</f>
+        <f t="shared" ref="DH5" si="34">DG5+1</f>
         <v>44840</v>
       </c>
       <c r="DI5" s="69">
-        <f t="shared" ref="DI5" ca="1" si="35">DH5+1</f>
+        <f t="shared" ref="DI5" si="35">DH5+1</f>
         <v>44841</v>
       </c>
       <c r="DJ5" s="69">
-        <f t="shared" ref="DJ5" ca="1" si="36">DI5+1</f>
+        <f t="shared" ref="DJ5" si="36">DI5+1</f>
         <v>44842</v>
       </c>
       <c r="DK5" s="70">
-        <f t="shared" ref="DK5" ca="1" si="37">DJ5+1</f>
+        <f t="shared" ref="DK5" si="37">DJ5+1</f>
         <v>44843</v>
       </c>
       <c r="DL5" s="68">
-        <f ca="1">DK5+1</f>
+        <f>DK5+1</f>
         <v>44844</v>
       </c>
       <c r="DM5" s="69">
-        <f ca="1">DL5+1</f>
+        <f>DL5+1</f>
         <v>44845</v>
       </c>
       <c r="DN5" s="69">
-        <f t="shared" ref="DN5" ca="1" si="38">DM5+1</f>
+        <f t="shared" ref="DN5" si="38">DM5+1</f>
         <v>44846</v>
       </c>
       <c r="DO5" s="69">
-        <f t="shared" ref="DO5" ca="1" si="39">DN5+1</f>
+        <f t="shared" ref="DO5" si="39">DN5+1</f>
         <v>44847</v>
       </c>
       <c r="DP5" s="69">
-        <f t="shared" ref="DP5" ca="1" si="40">DO5+1</f>
+        <f t="shared" ref="DP5" si="40">DO5+1</f>
         <v>44848</v>
       </c>
       <c r="DQ5" s="69">
-        <f t="shared" ref="DQ5" ca="1" si="41">DP5+1</f>
+        <f t="shared" ref="DQ5" si="41">DP5+1</f>
         <v>44849</v>
       </c>
       <c r="DR5" s="70">
-        <f t="shared" ref="DR5" ca="1" si="42">DQ5+1</f>
+        <f t="shared" ref="DR5" si="42">DQ5+1</f>
         <v>44850</v>
       </c>
       <c r="DS5" s="68">
-        <f ca="1">DR5+1</f>
+        <f>DR5+1</f>
         <v>44851</v>
       </c>
       <c r="DT5" s="69">
-        <f ca="1">DS5+1</f>
+        <f>DS5+1</f>
         <v>44852</v>
       </c>
       <c r="DU5" s="69">
-        <f t="shared" ref="DU5" ca="1" si="43">DT5+1</f>
+        <f t="shared" ref="DU5" si="43">DT5+1</f>
         <v>44853</v>
       </c>
       <c r="DV5" s="69">
-        <f t="shared" ref="DV5" ca="1" si="44">DU5+1</f>
+        <f t="shared" ref="DV5" si="44">DU5+1</f>
         <v>44854</v>
       </c>
       <c r="DW5" s="69">
-        <f t="shared" ref="DW5" ca="1" si="45">DV5+1</f>
+        <f t="shared" ref="DW5" si="45">DV5+1</f>
         <v>44855</v>
       </c>
       <c r="DX5" s="69">
-        <f t="shared" ref="DX5" ca="1" si="46">DW5+1</f>
+        <f t="shared" ref="DX5" si="46">DW5+1</f>
         <v>44856</v>
       </c>
       <c r="DY5" s="70">
-        <f t="shared" ref="DY5" ca="1" si="47">DX5+1</f>
+        <f t="shared" ref="DY5" si="47">DX5+1</f>
         <v>44857</v>
       </c>
       <c r="DZ5" s="68">
-        <f ca="1">DY5+1</f>
+        <f>DY5+1</f>
         <v>44858</v>
       </c>
       <c r="EA5" s="69">
-        <f ca="1">DZ5+1</f>
+        <f>DZ5+1</f>
         <v>44859</v>
       </c>
       <c r="EB5" s="69">
-        <f t="shared" ref="EB5" ca="1" si="48">EA5+1</f>
+        <f t="shared" ref="EB5" si="48">EA5+1</f>
         <v>44860</v>
       </c>
       <c r="EC5" s="69">
-        <f t="shared" ref="EC5" ca="1" si="49">EB5+1</f>
+        <f t="shared" ref="EC5" si="49">EB5+1</f>
         <v>44861</v>
       </c>
       <c r="ED5" s="69">
-        <f t="shared" ref="ED5" ca="1" si="50">EC5+1</f>
+        <f t="shared" ref="ED5" si="50">EC5+1</f>
         <v>44862</v>
       </c>
       <c r="EE5" s="69">
-        <f t="shared" ref="EE5" ca="1" si="51">ED5+1</f>
+        <f t="shared" ref="EE5" si="51">ED5+1</f>
         <v>44863</v>
       </c>
       <c r="EF5" s="70">
-        <f t="shared" ref="EF5" ca="1" si="52">EE5+1</f>
+        <f t="shared" ref="EF5" si="52">EE5+1</f>
         <v>44864</v>
       </c>
       <c r="EG5" s="68">
-        <f ca="1">EF5+1</f>
+        <f>EF5+1</f>
         <v>44865</v>
       </c>
       <c r="EH5" s="69">
-        <f ca="1">EG5+1</f>
+        <f>EG5+1</f>
         <v>44866</v>
       </c>
       <c r="EI5" s="69">
-        <f t="shared" ref="EI5" ca="1" si="53">EH5+1</f>
+        <f t="shared" ref="EI5" si="53">EH5+1</f>
         <v>44867</v>
       </c>
       <c r="EJ5" s="69">
-        <f t="shared" ref="EJ5" ca="1" si="54">EI5+1</f>
+        <f t="shared" ref="EJ5" si="54">EI5+1</f>
         <v>44868</v>
       </c>
       <c r="EK5" s="69">
-        <f t="shared" ref="EK5" ca="1" si="55">EJ5+1</f>
+        <f t="shared" ref="EK5" si="55">EJ5+1</f>
         <v>44869</v>
       </c>
       <c r="EL5" s="69">
-        <f t="shared" ref="EL5" ca="1" si="56">EK5+1</f>
+        <f t="shared" ref="EL5" si="56">EK5+1</f>
         <v>44870</v>
       </c>
       <c r="EM5" s="70">
-        <f t="shared" ref="EM5" ca="1" si="57">EL5+1</f>
+        <f t="shared" ref="EM5" si="57">EL5+1</f>
         <v>44871</v>
       </c>
       <c r="EN5" s="68">
-        <f ca="1">EM5+1</f>
+        <f>EM5+1</f>
         <v>44872</v>
       </c>
       <c r="EO5" s="69">
-        <f ca="1">EN5+1</f>
+        <f>EN5+1</f>
         <v>44873</v>
       </c>
       <c r="EP5" s="69">
-        <f t="shared" ref="EP5" ca="1" si="58">EO5+1</f>
+        <f t="shared" ref="EP5" si="58">EO5+1</f>
         <v>44874</v>
       </c>
       <c r="EQ5" s="69">
-        <f t="shared" ref="EQ5" ca="1" si="59">EP5+1</f>
+        <f t="shared" ref="EQ5" si="59">EP5+1</f>
         <v>44875</v>
       </c>
       <c r="ER5" s="69">
-        <f t="shared" ref="ER5" ca="1" si="60">EQ5+1</f>
+        <f t="shared" ref="ER5" si="60">EQ5+1</f>
         <v>44876</v>
       </c>
       <c r="ES5" s="69">
-        <f t="shared" ref="ES5" ca="1" si="61">ER5+1</f>
+        <f t="shared" ref="ES5" si="61">ER5+1</f>
         <v>44877</v>
       </c>
       <c r="ET5" s="70">
-        <f t="shared" ref="ET5" ca="1" si="62">ES5+1</f>
+        <f t="shared" ref="ET5" si="62">ES5+1</f>
         <v>44878</v>
       </c>
       <c r="EU5" s="68">
-        <f ca="1">ET5+1</f>
+        <f>ET5+1</f>
         <v>44879</v>
       </c>
       <c r="EV5" s="69">
-        <f ca="1">EU5+1</f>
+        <f>EU5+1</f>
         <v>44880</v>
       </c>
       <c r="EW5" s="69">
-        <f t="shared" ref="EW5" ca="1" si="63">EV5+1</f>
+        <f t="shared" ref="EW5" si="63">EV5+1</f>
         <v>44881</v>
       </c>
       <c r="EX5" s="69">
-        <f t="shared" ref="EX5" ca="1" si="64">EW5+1</f>
+        <f t="shared" ref="EX5" si="64">EW5+1</f>
         <v>44882</v>
       </c>
       <c r="EY5" s="69">
-        <f t="shared" ref="EY5" ca="1" si="65">EX5+1</f>
+        <f t="shared" ref="EY5" si="65">EX5+1</f>
         <v>44883</v>
       </c>
       <c r="EZ5" s="69">
-        <f t="shared" ref="EZ5" ca="1" si="66">EY5+1</f>
+        <f t="shared" ref="EZ5" si="66">EY5+1</f>
         <v>44884</v>
       </c>
       <c r="FA5" s="70">
-        <f t="shared" ref="FA5" ca="1" si="67">EZ5+1</f>
+        <f t="shared" ref="FA5" si="67">EZ5+1</f>
         <v>44885</v>
       </c>
     </row>
@@ -3281,591 +3281,591 @@
         <v>19</v>
       </c>
       <c r="K6" s="9" t="str">
-        <f t="shared" ref="K6" ca="1" si="68">LEFT(TEXT(K5,"ddd"),1)</f>
+        <f t="shared" ref="K6" si="68">LEFT(TEXT(K5,"ddd"),1)</f>
         <v>l</v>
       </c>
       <c r="L6" s="9" t="str">
-        <f t="shared" ref="L6:AT6" ca="1" si="69">LEFT(TEXT(L5,"ddd"),1)</f>
+        <f t="shared" ref="L6:AT6" si="69">LEFT(TEXT(L5,"ddd"),1)</f>
         <v>m</v>
       </c>
       <c r="M6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="N6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>j</v>
       </c>
       <c r="O6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>v</v>
       </c>
       <c r="P6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>s</v>
       </c>
       <c r="Q6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>d</v>
       </c>
       <c r="R6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>l</v>
       </c>
       <c r="S6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="T6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="U6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>j</v>
       </c>
       <c r="V6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>v</v>
       </c>
       <c r="W6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>s</v>
       </c>
       <c r="X6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>d</v>
       </c>
       <c r="Y6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>l</v>
       </c>
       <c r="Z6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="AA6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="AB6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>j</v>
       </c>
       <c r="AC6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>v</v>
       </c>
       <c r="AD6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>s</v>
       </c>
       <c r="AE6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>d</v>
       </c>
       <c r="AF6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>l</v>
       </c>
       <c r="AG6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="AH6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="AI6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>j</v>
       </c>
       <c r="AJ6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>v</v>
       </c>
       <c r="AK6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>s</v>
       </c>
       <c r="AL6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>d</v>
       </c>
       <c r="AM6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>l</v>
       </c>
       <c r="AN6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="AO6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>m</v>
       </c>
       <c r="AP6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>j</v>
       </c>
       <c r="AQ6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>v</v>
       </c>
       <c r="AR6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>s</v>
       </c>
       <c r="AS6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>d</v>
       </c>
       <c r="AT6" s="9" t="str">
-        <f t="shared" ca="1" si="69"/>
+        <f t="shared" si="69"/>
         <v>l</v>
       </c>
       <c r="AU6" s="9" t="str">
-        <f t="shared" ref="AU6:BM6" ca="1" si="70">LEFT(TEXT(AU5,"ddd"),1)</f>
+        <f t="shared" ref="AU6:BM6" si="70">LEFT(TEXT(AU5,"ddd"),1)</f>
         <v>m</v>
       </c>
       <c r="AV6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>m</v>
       </c>
       <c r="AW6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>j</v>
       </c>
       <c r="AX6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>v</v>
       </c>
       <c r="AY6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>s</v>
       </c>
       <c r="AZ6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>d</v>
       </c>
       <c r="BA6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>l</v>
       </c>
       <c r="BB6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>m</v>
       </c>
       <c r="BC6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>m</v>
       </c>
       <c r="BD6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>j</v>
       </c>
       <c r="BE6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>v</v>
       </c>
       <c r="BF6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>s</v>
       </c>
       <c r="BG6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>d</v>
       </c>
       <c r="BH6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>l</v>
       </c>
       <c r="BI6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>m</v>
       </c>
       <c r="BJ6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>m</v>
       </c>
       <c r="BK6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>j</v>
       </c>
       <c r="BL6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>v</v>
       </c>
       <c r="BM6" s="9" t="str">
-        <f t="shared" ca="1" si="70"/>
+        <f t="shared" si="70"/>
         <v>s</v>
       </c>
       <c r="BN6" s="9" t="str">
-        <f ca="1">LEFT(TEXT(BN5,"ddd"),1)</f>
+        <f>LEFT(TEXT(BN5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="BO6" s="9" t="str">
-        <f t="shared" ref="BO6:CH6" ca="1" si="71">LEFT(TEXT(BO5,"ddd"),1)</f>
+        <f t="shared" ref="BO6:CH6" si="71">LEFT(TEXT(BO5,"ddd"),1)</f>
         <v>l</v>
       </c>
       <c r="BP6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>m</v>
       </c>
       <c r="BQ6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>m</v>
       </c>
       <c r="BR6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>j</v>
       </c>
       <c r="BS6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>v</v>
       </c>
       <c r="BT6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>s</v>
       </c>
       <c r="BU6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>d</v>
       </c>
       <c r="BV6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>l</v>
       </c>
       <c r="BW6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>m</v>
       </c>
       <c r="BX6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>m</v>
       </c>
       <c r="BY6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>j</v>
       </c>
       <c r="BZ6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>v</v>
       </c>
       <c r="CA6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>s</v>
       </c>
       <c r="CB6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>d</v>
       </c>
       <c r="CC6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>l</v>
       </c>
       <c r="CD6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>m</v>
       </c>
       <c r="CE6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>m</v>
       </c>
       <c r="CF6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>j</v>
       </c>
       <c r="CG6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>v</v>
       </c>
       <c r="CH6" s="9" t="str">
-        <f t="shared" ca="1" si="71"/>
+        <f t="shared" si="71"/>
         <v>s</v>
       </c>
       <c r="CI6" s="9" t="str">
-        <f ca="1">LEFT(TEXT(CI5,"ddd"),1)</f>
+        <f>LEFT(TEXT(CI5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="CJ6" s="9" t="str">
-        <f t="shared" ref="CJ6:DC6" ca="1" si="72">LEFT(TEXT(CJ5,"ddd"),1)</f>
+        <f t="shared" ref="CJ6:DC6" si="72">LEFT(TEXT(CJ5,"ddd"),1)</f>
         <v>l</v>
       </c>
       <c r="CK6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>m</v>
       </c>
       <c r="CL6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>m</v>
       </c>
       <c r="CM6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>j</v>
       </c>
       <c r="CN6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>v</v>
       </c>
       <c r="CO6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>s</v>
       </c>
       <c r="CP6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>d</v>
       </c>
       <c r="CQ6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>l</v>
       </c>
       <c r="CR6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>m</v>
       </c>
       <c r="CS6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>m</v>
       </c>
       <c r="CT6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>j</v>
       </c>
       <c r="CU6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>v</v>
       </c>
       <c r="CV6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>s</v>
       </c>
       <c r="CW6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>d</v>
       </c>
       <c r="CX6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>l</v>
       </c>
       <c r="CY6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>m</v>
       </c>
       <c r="CZ6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>m</v>
       </c>
       <c r="DA6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>j</v>
       </c>
       <c r="DB6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>v</v>
       </c>
       <c r="DC6" s="9" t="str">
-        <f t="shared" ca="1" si="72"/>
+        <f t="shared" si="72"/>
         <v>s</v>
       </c>
       <c r="DD6" s="9" t="str">
-        <f ca="1">LEFT(TEXT(DD5,"ddd"),1)</f>
+        <f>LEFT(TEXT(DD5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="DE6" s="9" t="str">
-        <f t="shared" ref="DE6:DX6" ca="1" si="73">LEFT(TEXT(DE5,"ddd"),1)</f>
+        <f t="shared" ref="DE6:DX6" si="73">LEFT(TEXT(DE5,"ddd"),1)</f>
         <v>l</v>
       </c>
       <c r="DF6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>m</v>
       </c>
       <c r="DG6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>m</v>
       </c>
       <c r="DH6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>j</v>
       </c>
       <c r="DI6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>v</v>
       </c>
       <c r="DJ6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>s</v>
       </c>
       <c r="DK6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>d</v>
       </c>
       <c r="DL6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>l</v>
       </c>
       <c r="DM6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>m</v>
       </c>
       <c r="DN6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>m</v>
       </c>
       <c r="DO6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>j</v>
       </c>
       <c r="DP6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>v</v>
       </c>
       <c r="DQ6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>s</v>
       </c>
       <c r="DR6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>d</v>
       </c>
       <c r="DS6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>l</v>
       </c>
       <c r="DT6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>m</v>
       </c>
       <c r="DU6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>m</v>
       </c>
       <c r="DV6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>j</v>
       </c>
       <c r="DW6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>v</v>
       </c>
       <c r="DX6" s="9" t="str">
-        <f t="shared" ca="1" si="73"/>
+        <f t="shared" si="73"/>
         <v>s</v>
       </c>
       <c r="DY6" s="9" t="str">
-        <f ca="1">LEFT(TEXT(DY5,"ddd"),1)</f>
+        <f>LEFT(TEXT(DY5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="DZ6" s="9" t="str">
-        <f t="shared" ref="DZ6:ES6" ca="1" si="74">LEFT(TEXT(DZ5,"ddd"),1)</f>
+        <f t="shared" ref="DZ6:ES6" si="74">LEFT(TEXT(DZ5,"ddd"),1)</f>
         <v>l</v>
       </c>
       <c r="EA6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>m</v>
       </c>
       <c r="EB6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>m</v>
       </c>
       <c r="EC6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>j</v>
       </c>
       <c r="ED6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>v</v>
       </c>
       <c r="EE6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>s</v>
       </c>
       <c r="EF6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>d</v>
       </c>
       <c r="EG6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>l</v>
       </c>
       <c r="EH6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>m</v>
       </c>
       <c r="EI6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>m</v>
       </c>
       <c r="EJ6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>j</v>
       </c>
       <c r="EK6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>v</v>
       </c>
       <c r="EL6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>s</v>
       </c>
       <c r="EM6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>d</v>
       </c>
       <c r="EN6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>l</v>
       </c>
       <c r="EO6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>m</v>
       </c>
       <c r="EP6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>m</v>
       </c>
       <c r="EQ6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>j</v>
       </c>
       <c r="ER6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>v</v>
       </c>
       <c r="ES6" s="9" t="str">
-        <f t="shared" ca="1" si="74"/>
+        <f t="shared" si="74"/>
         <v>s</v>
       </c>
       <c r="ET6" s="9" t="str">
-        <f ca="1">LEFT(TEXT(ET5,"ddd"),1)</f>
+        <f>LEFT(TEXT(ET5,"ddd"),1)</f>
         <v>d</v>
       </c>
       <c r="EU6" s="9" t="str">
-        <f t="shared" ref="EU6:EZ6" ca="1" si="75">LEFT(TEXT(EU5,"ddd"),1)</f>
+        <f t="shared" ref="EU6:EZ6" si="75">LEFT(TEXT(EU5,"ddd"),1)</f>
         <v>l</v>
       </c>
       <c r="EV6" s="9" t="str">
-        <f t="shared" ca="1" si="75"/>
+        <f t="shared" si="75"/>
         <v>m</v>
       </c>
       <c r="EW6" s="9" t="str">
-        <f t="shared" ca="1" si="75"/>
+        <f t="shared" si="75"/>
         <v>m</v>
       </c>
       <c r="EX6" s="9" t="str">
-        <f t="shared" ca="1" si="75"/>
+        <f t="shared" si="75"/>
         <v>j</v>
       </c>
       <c r="EY6" s="9" t="str">
-        <f t="shared" ca="1" si="75"/>
+        <f t="shared" si="75"/>
         <v>v</v>
       </c>
       <c r="EZ6" s="9" t="str">
-        <f t="shared" ca="1" si="75"/>
+        <f t="shared" si="75"/>
         <v>s</v>
       </c>
       <c r="FA6" s="9" t="str">
-        <f ca="1">LEFT(TEXT(FA5,"ddd"),1)</f>
+        <f>LEFT(TEXT(FA5,"ddd"),1)</f>
         <v>d</v>
       </c>
     </row>
@@ -4210,19 +4210,19 @@
         <v>53</v>
       </c>
       <c r="F9" s="13">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="59">
-        <f ca="1">Inicio_del_proyecto</f>
-        <v>44740</v>
+        <f>Inicio_del_proyecto</f>
+        <v>44743</v>
       </c>
       <c r="H9" s="59">
-        <f ca="1">G9+14</f>
-        <v>44754</v>
+        <f>G9+14</f>
+        <v>44757</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K9" s="22"/>
@@ -4391,16 +4391,16 @@
         <v>0</v>
       </c>
       <c r="G10" s="59">
-        <f ca="1">Inicio_del_proyecto</f>
-        <v>44740</v>
+        <f>Inicio_del_proyecto</f>
+        <v>44743</v>
       </c>
       <c r="H10" s="59">
-        <f t="shared" ref="H10:H12" ca="1" si="77">G10+14</f>
-        <v>44754</v>
+        <f t="shared" ref="H10:H12" si="77">G10+14</f>
+        <v>44757</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K10" s="22"/>
@@ -4567,16 +4567,16 @@
         <v>0</v>
       </c>
       <c r="G11" s="59">
-        <f ca="1">Inicio_del_proyecto</f>
-        <v>44740</v>
+        <f>Inicio_del_proyecto</f>
+        <v>44743</v>
       </c>
       <c r="H11" s="59">
-        <f t="shared" ca="1" si="77"/>
-        <v>44754</v>
+        <f t="shared" si="77"/>
+        <v>44757</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K11" s="22"/>
@@ -4743,16 +4743,16 @@
         <v>0</v>
       </c>
       <c r="G12" s="59">
-        <f ca="1">Inicio_del_proyecto</f>
-        <v>44740</v>
+        <f>Inicio_del_proyecto</f>
+        <v>44743</v>
       </c>
       <c r="H12" s="59">
-        <f t="shared" ca="1" si="77"/>
-        <v>44754</v>
+        <f t="shared" si="77"/>
+        <v>44757</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K12" s="22"/>
@@ -5247,16 +5247,16 @@
         <v>0</v>
       </c>
       <c r="G15" s="59">
-        <f ca="1">Inicio_del_proyecto+21</f>
-        <v>44761</v>
+        <f>Inicio_del_proyecto+21</f>
+        <v>44764</v>
       </c>
       <c r="H15" s="62">
-        <f ca="1">G15+7</f>
-        <v>44768</v>
+        <f>G15+7</f>
+        <v>44771</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>8</v>
       </c>
       <c r="K15" s="22"/>
@@ -5422,16 +5422,16 @@
         <v>0</v>
       </c>
       <c r="G16" s="59">
-        <f ca="1">H15</f>
-        <v>44768</v>
+        <f>H15</f>
+        <v>44771</v>
       </c>
       <c r="H16" s="62">
-        <f ca="1">G16+7</f>
-        <v>44775</v>
+        <f>G16+7</f>
+        <v>44778</v>
       </c>
       <c r="I16" s="10"/>
       <c r="J16" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>8</v>
       </c>
       <c r="K16" s="22"/>
@@ -5598,16 +5598,16 @@
         <v>0</v>
       </c>
       <c r="G17" s="59">
-        <f ca="1">H16</f>
-        <v>44775</v>
+        <f>H16</f>
+        <v>44778</v>
       </c>
       <c r="H17" s="62">
-        <f ca="1">G17+7</f>
-        <v>44782</v>
+        <f>G17+7</f>
+        <v>44785</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>8</v>
       </c>
       <c r="K17" s="22"/>
@@ -6262,16 +6262,16 @@
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="59">
-        <f ca="1">Inicio_del_proyecto</f>
-        <v>44740</v>
+        <f>Inicio_del_proyecto</f>
+        <v>44743</v>
       </c>
       <c r="H21" s="65">
-        <f ca="1">G21+14</f>
-        <v>44754</v>
+        <f>G21+14</f>
+        <v>44757</v>
       </c>
       <c r="I21" s="10"/>
       <c r="J21" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K21" s="22"/>
@@ -6436,16 +6436,16 @@
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="65">
-        <f ca="1">H21</f>
-        <v>44754</v>
+        <f>H21</f>
+        <v>44757</v>
       </c>
       <c r="H22" s="65">
-        <f ca="1">G22+30</f>
-        <v>44784</v>
+        <f>G22+30</f>
+        <v>44787</v>
       </c>
       <c r="I22" s="10"/>
       <c r="J22" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>31</v>
       </c>
       <c r="K22" s="22"/>
@@ -6610,16 +6610,16 @@
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="59">
-        <f ca="1">Inicio_del_proyecto+37</f>
-        <v>44777</v>
+        <f>Inicio_del_proyecto+37</f>
+        <v>44780</v>
       </c>
       <c r="H23" s="65">
-        <f ca="1">G23+30</f>
-        <v>44807</v>
+        <f>G23+30</f>
+        <v>44810</v>
       </c>
       <c r="I23" s="10"/>
       <c r="J23" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>31</v>
       </c>
       <c r="K23" s="22"/>
@@ -6784,16 +6784,16 @@
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="59">
-        <f ca="1">Inicio_del_proyecto+37</f>
-        <v>44777</v>
+        <f>Inicio_del_proyecto+37</f>
+        <v>44780</v>
       </c>
       <c r="H24" s="65">
-        <f ca="1">G24+30</f>
-        <v>44807</v>
+        <f>G24+30</f>
+        <v>44810</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>31</v>
       </c>
       <c r="K24" s="22"/>
@@ -6958,16 +6958,16 @@
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="59">
-        <f ca="1">Inicio_del_proyecto+67</f>
-        <v>44807</v>
+        <f>Inicio_del_proyecto+67</f>
+        <v>44810</v>
       </c>
       <c r="H25" s="65">
-        <f ca="1">G25+30</f>
-        <v>44837</v>
+        <f>G25+30</f>
+        <v>44840</v>
       </c>
       <c r="I25" s="10"/>
       <c r="J25" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>31</v>
       </c>
       <c r="K25" s="22"/>
@@ -7300,16 +7300,16 @@
         <v>0</v>
       </c>
       <c r="G27" s="59">
-        <f ca="1">Inicio_del_proyecto+40</f>
-        <v>44780</v>
+        <f>Inicio_del_proyecto+40</f>
+        <v>44783</v>
       </c>
       <c r="H27" s="59">
-        <f ca="1">G27+14</f>
-        <v>44794</v>
+        <f>G27+14</f>
+        <v>44797</v>
       </c>
       <c r="I27" s="10"/>
       <c r="J27" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K27" s="22"/>
@@ -7476,16 +7476,16 @@
         <v>0</v>
       </c>
       <c r="G28" s="59">
-        <f ca="1">Inicio_del_proyecto+40</f>
-        <v>44780</v>
+        <f>Inicio_del_proyecto+40</f>
+        <v>44783</v>
       </c>
       <c r="H28" s="59">
-        <f ca="1">G28+21</f>
-        <v>44801</v>
+        <f>G28+21</f>
+        <v>44804</v>
       </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>22</v>
       </c>
       <c r="K28" s="22"/>
@@ -7652,16 +7652,16 @@
         <v>0</v>
       </c>
       <c r="G29" s="59">
-        <f ca="1">H28</f>
-        <v>44801</v>
+        <f>H28</f>
+        <v>44804</v>
       </c>
       <c r="H29" s="59">
-        <f ca="1">G29+21</f>
-        <v>44822</v>
+        <f>G29+21</f>
+        <v>44825</v>
       </c>
       <c r="I29" s="10"/>
       <c r="J29" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>22</v>
       </c>
       <c r="K29" s="22"/>
@@ -7828,16 +7828,16 @@
         <v>0</v>
       </c>
       <c r="G30" s="59">
-        <f ca="1">H29</f>
-        <v>44822</v>
+        <f>H29</f>
+        <v>44825</v>
       </c>
       <c r="H30" s="59">
-        <f ca="1">G30+14</f>
-        <v>44836</v>
+        <f>G30+14</f>
+        <v>44839</v>
       </c>
       <c r="I30" s="10"/>
       <c r="J30" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K30" s="22"/>
@@ -8004,16 +8004,16 @@
         <v>0</v>
       </c>
       <c r="G31" s="59">
-        <f ca="1">H27</f>
-        <v>44794</v>
+        <f>H27</f>
+        <v>44797</v>
       </c>
       <c r="H31" s="59">
-        <f ca="1">G31+14</f>
-        <v>44808</v>
+        <f>G31+14</f>
+        <v>44811</v>
       </c>
       <c r="I31" s="10"/>
       <c r="J31" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K31" s="22"/>
@@ -8509,16 +8509,16 @@
         <v>0</v>
       </c>
       <c r="G34" s="59">
-        <f ca="1">Inicio_del_proyecto+60</f>
-        <v>44800</v>
+        <f>Inicio_del_proyecto+60</f>
+        <v>44803</v>
       </c>
       <c r="H34" s="59">
-        <f ca="1">G34+14</f>
-        <v>44814</v>
+        <f>G34+14</f>
+        <v>44817</v>
       </c>
       <c r="I34" s="10"/>
       <c r="J34" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K34" s="22"/>
@@ -8684,16 +8684,16 @@
         <v>0</v>
       </c>
       <c r="G35" s="59">
-        <f ca="1">Inicio_del_proyecto+60</f>
-        <v>44800</v>
+        <f>Inicio_del_proyecto+60</f>
+        <v>44803</v>
       </c>
       <c r="H35" s="59">
-        <f t="shared" ref="H35:H37" ca="1" si="78">G35+14</f>
-        <v>44814</v>
+        <f t="shared" ref="H35:H37" si="78">G35+14</f>
+        <v>44817</v>
       </c>
       <c r="I35" s="10"/>
       <c r="J35" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K35" s="22"/>
@@ -8859,16 +8859,16 @@
         <v>0</v>
       </c>
       <c r="G36" s="59">
-        <f ca="1">Inicio_del_proyecto+60</f>
-        <v>44800</v>
+        <f>Inicio_del_proyecto+60</f>
+        <v>44803</v>
       </c>
       <c r="H36" s="59">
-        <f t="shared" ca="1" si="78"/>
-        <v>44814</v>
+        <f t="shared" si="78"/>
+        <v>44817</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K36" s="22"/>
@@ -9034,16 +9034,16 @@
         <v>0</v>
       </c>
       <c r="G37" s="59">
-        <f ca="1">Inicio_del_proyecto+60</f>
-        <v>44800</v>
+        <f>Inicio_del_proyecto+60</f>
+        <v>44803</v>
       </c>
       <c r="H37" s="59">
-        <f t="shared" ca="1" si="78"/>
-        <v>44814</v>
+        <f t="shared" si="78"/>
+        <v>44817</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10">
-        <f t="shared" ca="1" si="76"/>
+        <f t="shared" si="76"/>
         <v>15</v>
       </c>
       <c r="K37" s="22"/>

</xml_diff>